<commit_message>
fix bugs with remainder count
</commit_message>
<xml_diff>
--- a/mediafiles/release_mat_stats.xlsx
+++ b/mediafiles/release_mat_stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>#</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Работа</t>
   </si>
   <si>
-    <t>Количество</t>
-  </si>
-  <si>
     <t>Отпущено</t>
   </si>
   <si>
@@ -60,6 +57,12 @@
   </si>
   <si>
     <t>Возврат</t>
+  </si>
+  <si>
+    <t>Количество(Общее)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество (Были) </t>
   </si>
 </sst>
 </file>
@@ -485,76 +488,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>